<commit_message>
[Update] Add in cahier labo comments
</commit_message>
<xml_diff>
--- a/CahierLaboMagninMetthez.xlsx
+++ b/CahierLaboMagninMetthez.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="11_AD4DB114E441178AC67DF437FE92CEEE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE5A6375-2D24-4713-BD35-F846D5FD2FBD}"/>
+  <xr:revisionPtr revIDLastSave="368" documentId="11_AD4DB114E441178AC67DF437FE92CEEE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF07499E-E61A-4757-AB20-CF10AFF5EF6B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t>Qui ?</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Tester le Programme</t>
+  </si>
+  <si>
+    <t>Ces nouveaux opcodes permetteront de faire des "fonctions", des "pointeurs" et des "tableaux"</t>
   </si>
 </sst>
 </file>
@@ -618,36 +621,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -671,6 +644,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,7 +964,7 @@
   <dimension ref="B2:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,10 +975,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -992,12 +995,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -1028,12 +1031,12 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
@@ -1114,12 +1117,12 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
@@ -1176,12 +1179,12 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
     </row>
     <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
@@ -1244,12 +1247,12 @@
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
@@ -1314,12 +1317,12 @@
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
@@ -1358,156 +1361,158 @@
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="20"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="31"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="31">
+      <c r="D36" s="21">
         <v>3.125E-2</v>
       </c>
-      <c r="E36" s="30"/>
+      <c r="E36" s="20"/>
     </row>
     <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="30"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="20"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="30"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="20"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="31">
+      <c r="D39" s="21">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E39" s="30"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="40" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="30"/>
+      <c r="C40" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="18"/>
+      <c r="E40" s="20"/>
     </row>
     <row r="41" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="31">
+      <c r="C41" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="21">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E41" s="34"/>
-    </row>
-    <row r="42" spans="2:5" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="32" t="s">
+      <c r="E41" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="36"/>
-      <c r="E42" s="34"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="24"/>
     </row>
     <row r="43" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="31">
+      <c r="D43" s="21">
         <v>0.20833333333333334</v>
       </c>
-      <c r="E43" s="34"/>
+      <c r="E43" s="24"/>
     </row>
     <row r="44" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="34"/>
+      <c r="C44" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="21"/>
+      <c r="E44" s="24"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="31">
+      <c r="C45" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="21">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E45" s="34"/>
+      <c r="E45" s="24"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="31"/>
-      <c r="E46" s="34"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="24"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="32"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="34"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="24"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="32"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="34"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="24"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="32"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="34"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="24"/>
     </row>
     <row r="50" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="33"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="14"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="35"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
[Update] Modify CahierLoba following group discussion
</commit_message>
<xml_diff>
--- a/CahierLaboMagninMetthez.xlsx
+++ b/CahierLaboMagninMetthez.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="368" documentId="11_AD4DB114E441178AC67DF437FE92CEEE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF07499E-E61A-4757-AB20-CF10AFF5EF6B}"/>
+  <xr:revisionPtr revIDLastSave="382" documentId="11_AD4DB114E441178AC67DF437FE92CEEE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{937FB1FD-D3F6-44FC-8395-43CA84BC78BB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>Qui ?</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Test concept sur le projet vivado</t>
   </si>
   <si>
-    <t>Ajouter les nouveaux opcode dans le document sorties séquenceur</t>
-  </si>
-  <si>
     <t>Faire les modifications document sorties séquenceur et dans le jeux d'instruction en conséquence</t>
   </si>
   <si>
@@ -208,6 +205,15 @@
   </si>
   <si>
     <t>Ces nouveaux opcodes permetteront de faire des "fonctions", des "pointeurs" et des "tableaux"</t>
+  </si>
+  <si>
+    <t>Implémentation des opcodes afin de vérifier le bon fonctionnement.</t>
+  </si>
+  <si>
+    <t>Ajouter les nouveaux opcodes dans le document sorties séquenceur</t>
+  </si>
+  <si>
+    <t>La grande partie du travail était les opcodes que nous avons décidé d'ajouter.</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -673,6 +679,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,8 +972,8 @@
   </sheetPr>
   <dimension ref="B2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,12 +1391,14 @@
     </row>
     <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="22" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="18"/>
+      <c r="D37" s="21">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E37" s="20"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -1397,7 +1408,9 @@
       <c r="C38" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="18"/>
+      <c r="D38" s="21">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E38" s="20"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -1405,26 +1418,30 @@
         <v>47</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D39" s="21">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E39" s="20"/>
+      <c r="E39" s="20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="40" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="18"/>
+      <c r="D40" s="21">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E40" s="20"/>
     </row>
     <row r="41" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>5</v>
@@ -1433,22 +1450,24 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="2:5" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="26"/>
+      <c r="D42" s="39">
+        <v>3.125E-2</v>
+      </c>
       <c r="E42" s="24"/>
     </row>
     <row r="43" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>16</v>
@@ -1456,21 +1475,25 @@
       <c r="D43" s="21">
         <v>0.20833333333333334</v>
       </c>
-      <c r="E43" s="24"/>
+      <c r="E43" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="44" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="21"/>
+      <c r="D44" s="21">
+        <v>3.125E-2</v>
+      </c>
       <c r="E44" s="24"/>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>5</v>
@@ -1482,12 +1505,14 @@
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="21"/>
+      <c r="D46" s="21">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="E46" s="24"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Update] New cahier entry$
</commit_message>
<xml_diff>
--- a/CahierLaboMagninMetthez.xlsx
+++ b/CahierLaboMagninMetthez.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS\sysnumapp\NanoProcessor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2953AE-BD23-44B6-BF53-57F0E43DC5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176542A5-82CA-4DAE-BEA0-3EDA7403C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
   <si>
     <t>Qui ?</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>Faire le programme "assembleur" pour le rendu 4 en utilisant des sauts-routines</t>
+  </si>
+  <si>
+    <t>Ajout des leds bicolores dans la ROM</t>
+  </si>
+  <si>
+    <t>Adaptation du testbench pour les leds</t>
+  </si>
+  <si>
+    <t>Il nous a semblé que le fichier excel pour faire le fichier de contraintes comportait une erreur pour les leds bicolores (inversion). Un peu de temps a été perdu dans la confusion.</t>
   </si>
 </sst>
 </file>
@@ -582,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -628,8 +637,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -643,16 +650,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -682,6 +683,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,7 +976,7 @@
   <dimension ref="B2:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,10 +987,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1000,12 +1007,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
@@ -1036,12 +1043,12 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="39"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
@@ -1122,12 +1129,12 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
@@ -1184,12 +1191,12 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
@@ -1252,12 +1259,12 @@
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
@@ -1322,12 +1329,12 @@
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
@@ -1366,109 +1373,109 @@
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="32"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="6">
         <v>3.125E-2</v>
       </c>
-      <c r="E36" s="20"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="6">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E37" s="20"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="6">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="21">
+      <c r="C39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="21">
+      <c r="C40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E40" s="20"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="21">
+      <c r="C41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="6">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="2:5" s="27" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="22" t="s">
+    <row r="42" spans="2:5" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42" s="37">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E42" s="24"/>
+      <c r="E42" s="8"/>
     </row>
     <row r="43" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="21">
+      <c r="D43" s="6">
         <v>0.20833333333333334</v>
       </c>
       <c r="E43" s="8" t="s">
@@ -1476,64 +1483,78 @@
       </c>
     </row>
     <row r="44" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="21">
+      <c r="C44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="6">
         <v>3.125E-2</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="21">
+      <c r="C45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E45" s="24"/>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="21">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E46" s="24"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="22"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="24"/>
+      <c r="D46" s="6">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B47" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="6">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="22"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="24"/>
+      <c r="B48" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="6">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E48" s="8"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="22"/>
+      <c r="B49" s="20"/>
       <c r="C49" s="18"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="24"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="22"/>
     </row>
     <row r="50" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="23"/>
+      <c r="B50" s="21"/>
       <c r="C50" s="14"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
[Update] New cahier entry
</commit_message>
<xml_diff>
--- a/CahierLaboMagninMetthez.xlsx
+++ b/CahierLaboMagninMetthez.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS\sysnumapp\NanoProcessor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176542A5-82CA-4DAE-BEA0-3EDA7403C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC81BC2-BD39-44E0-B540-3963F36906BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
   <si>
     <t>Qui ?</t>
   </si>
@@ -147,9 +147,6 @@
 Permettra de garantir l'intégrité et l'authenticité de notre travail.</t>
   </si>
   <si>
-    <t>Ccomprendre le cahier du rendu 3</t>
-  </si>
-  <si>
     <t>Créer des issues pour organiser notre travail</t>
   </si>
   <si>
@@ -223,6 +220,15 @@
   </si>
   <si>
     <t>Il nous a semblé que le fichier excel pour faire le fichier de contraintes comportait une erreur pour les leds bicolores (inversion). Un peu de temps a été perdu dans la confusion.</t>
+  </si>
+  <si>
+    <t>27.04.2023</t>
+  </si>
+  <si>
+    <t>Comprendre le cahier du rendu 3</t>
+  </si>
+  <si>
+    <t>Création des pdfs pour le rendu 3</t>
   </si>
 </sst>
 </file>
@@ -591,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -654,6 +660,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -684,10 +696,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -973,10 +988,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:E50"/>
+  <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,10 +1002,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1007,12 +1022,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
@@ -1043,12 +1058,12 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
@@ -1129,12 +1144,12 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
@@ -1191,12 +1206,12 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
@@ -1259,12 +1274,12 @@
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
@@ -1280,10 +1295,10 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="D27" s="17">
         <v>1.0416666666666666E-2</v>
@@ -1306,7 +1321,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>5</v>
@@ -1318,7 +1333,7 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>5</v>
@@ -1329,16 +1344,16 @@
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="28"/>
+      <c r="B31" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="30"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>5</v>
@@ -1350,7 +1365,7 @@
     </row>
     <row r="33" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>5</v>
@@ -1362,7 +1377,7 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>5</v>
@@ -1373,16 +1388,16 @@
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
+      <c r="B35" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="30"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>16</v>
@@ -1394,7 +1409,7 @@
     </row>
     <row r="37" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>14</v>
@@ -1406,7 +1421,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>14</v>
@@ -1418,7 +1433,7 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>5</v>
@@ -1427,12 +1442,12 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>5</v>
@@ -1444,7 +1459,7 @@
     </row>
     <row r="41" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>5</v>
@@ -1453,24 +1468,24 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="2:5" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="37">
+      <c r="D42" s="27">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E42" s="8"/>
     </row>
     <row r="43" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>16</v>
@@ -1479,12 +1494,12 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>5</v>
@@ -1496,7 +1511,7 @@
     </row>
     <row r="45" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>5</v>
@@ -1508,7 +1523,7 @@
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>14</v>
@@ -1520,7 +1535,7 @@
     </row>
     <row r="47" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>5</v>
@@ -1529,12 +1544,12 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>5</v>
@@ -1545,19 +1560,34 @@
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="20"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="22"/>
-    </row>
-    <row r="50" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="21"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="23"/>
+      <c r="B49" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="40"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="19">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E50" s="22"/>
+    </row>
+    <row r="51" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="21"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B49:E49"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B25:E25"/>
@@ -1568,6 +1598,6 @@
     <mergeCell ref="B14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="68" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="67" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Modify] Correct cahier labo before to return
</commit_message>
<xml_diff>
--- a/CahierLaboMagninMetthez.xlsx
+++ b/CahierLaboMagninMetthez.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS\sysnumapp\NanoProcessor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC81BC2-BD39-44E0-B540-3963F36906BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{5EC81BC2-BD39-44E0-B540-3963F36906BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A89B5091-8794-4C7C-B39A-7AD3A876C819}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -642,15 +642,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -667,6 +659,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -695,15 +696,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,26 +980,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:E51"/>
+  <dimension ref="B2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1021,15 +1013,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="32" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
@@ -1043,7 +1035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1057,15 +1049,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="35" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="37"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1079,7 +1071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1093,7 +1085,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1105,7 +1097,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1117,7 +1109,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
@@ -1129,7 +1121,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1143,15 +1135,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="28" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1157,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1171,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1191,7 +1183,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>24</v>
       </c>
@@ -1205,15 +1197,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="28" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>26</v>
       </c>
@@ -1225,7 +1217,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
@@ -1237,7 +1229,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
@@ -1249,7 +1241,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>29</v>
       </c>
@@ -1261,7 +1253,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
@@ -1273,15 +1265,15 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="28" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>32</v>
       </c>
@@ -1293,7 +1285,7 @@
       </c>
       <c r="E26" s="13"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>37</v>
       </c>
@@ -1305,7 +1297,7 @@
       </c>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>34</v>
       </c>
@@ -1319,7 +1311,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>62</v>
       </c>
@@ -1331,7 +1323,7 @@
       </c>
       <c r="E29" s="16"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
@@ -1343,15 +1335,15 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="28" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>40</v>
       </c>
@@ -1363,7 +1355,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
         <v>42</v>
       </c>
@@ -1375,7 +1367,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>41</v>
       </c>
@@ -1387,15 +1379,15 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="28" t="s">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="29"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>44</v>
       </c>
@@ -1407,7 +1399,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
         <v>55</v>
       </c>
@@ -1419,7 +1411,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>45</v>
       </c>
@@ -1431,7 +1423,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>46</v>
       </c>
@@ -1445,7 +1437,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>47</v>
       </c>
@@ -1457,7 +1449,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>48</v>
       </c>
@@ -1471,19 +1463,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="2:5" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="27">
+      <c r="D42" s="23">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
         <v>51</v>
       </c>
@@ -1497,7 +1489,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
         <v>50</v>
       </c>
@@ -1509,7 +1501,7 @@
       </c>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="9" t="s">
         <v>57</v>
       </c>
@@ -1521,7 +1513,7 @@
       </c>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
         <v>52</v>
       </c>
@@ -1533,7 +1525,7 @@
       </c>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
         <v>58</v>
       </c>
@@ -1547,7 +1539,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
         <v>59</v>
       </c>
@@ -1559,43 +1551,37 @@
       </c>
       <c r="E48" s="8"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="38" t="s">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="40"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="20" t="s">
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="26"/>
+    </row>
+    <row r="50" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="19">
+      <c r="D50" s="21">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E50" s="22"/>
-    </row>
-    <row r="51" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="21"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="23"/>
+      <c r="E50" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B49:E49"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="67" orientation="portrait" r:id="rId1"/>

</xml_diff>